<commit_message>
Submit New Usecase Description
</commit_message>
<xml_diff>
--- a/SUBMIT_PLACE/MINH_DOAN/REQUIREMENT/Assign Requirement Task.xlsx
+++ b/SUBMIT_PLACE/MINH_DOAN/REQUIREMENT/Assign Requirement Task.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>No.</t>
   </si>
@@ -79,15 +79,6 @@
   </si>
   <si>
     <t>21h 15/1/2017</t>
-  </si>
-  <si>
-    <t>21h 15/1/2018</t>
-  </si>
-  <si>
-    <t>21h 15/1/2019</t>
-  </si>
-  <si>
-    <t>21h 15/1/2020</t>
   </si>
   <si>
     <t>Context Diagram cần xem lại Function List của Hải sửa để vẽ lại</t>
@@ -359,9 +350,6 @@
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -372,20 +360,23 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -693,7 +684,7 @@
   <dimension ref="E2:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,172 +699,172 @@
   </cols>
   <sheetData>
     <row r="2" spans="5:9" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
     </row>
     <row r="3" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="5:9" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="5:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>1</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="9"/>
+      <c r="I5" s="8"/>
     </row>
     <row r="6" spans="5:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>2</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="5:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E7" s="5">
+        <v>3</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="5:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E8" s="5">
+        <v>4</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" spans="5:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E9" s="5">
+        <v>5</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="5:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E10" s="17">
+        <v>6</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="5:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E11" s="17"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="5:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E12" s="17"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="5:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E13" s="18"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="13" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="5:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E7" s="6">
-        <v>3</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="5:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E8" s="6">
-        <v>4</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" spans="5:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E9" s="6">
-        <v>5</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="5:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E10" s="13">
-        <v>6</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="5:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E11" s="13"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="5:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="5:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E13" s="15"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I13" s="18" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="16" spans="5:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F16" s="19" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G16" s="19"/>
       <c r="H16" s="19"/>

</xml_diff>